<commit_message>
Updated templates and export functions
</commit_message>
<xml_diff>
--- a/frontend-next/public/templates/gob_template.xlsx
+++ b/frontend-next/public/templates/gob_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Egresados</t>
   </si>
@@ -29,10 +29,13 @@
     <t xml:space="preserve">Titulados</t>
   </si>
   <si>
-    <t xml:space="preserve">{results.year}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{results.count}</t>
+    <t xml:space="preserve">{summary.year}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{summary.graduates}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{summary.titles}</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -205,40 +208,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -493,41 +500,43 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -547,175 +556,175 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="32.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="30.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="42.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="27.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="5" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="32.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="30.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="42.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="27.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="6" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
+      <c r="D9" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>